<commit_message>
#3 added test harness for login and added login fixed.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -26,56 +26,64 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>RickG</t>
-  </si>
-  <si>
-    <t>Zatu6226</t>
-  </si>
-  <si>
-    <t>DarylD</t>
-  </si>
-  <si>
     <t>Labo0749</t>
   </si>
   <si>
-    <t>Michonne</t>
-  </si>
-  <si>
     <t>Zuwu5875</t>
   </si>
   <si>
-    <t>CarlG</t>
-  </si>
-  <si>
     <t>Pufa7292</t>
   </si>
   <si>
-    <t>GlennR</t>
-  </si>
-  <si>
     <t>Hoyo4800</t>
   </si>
   <si>
-    <t>MaggieG</t>
-  </si>
-  <si>
     <t>Puva8501</t>
   </si>
   <si>
-    <t>HershelG</t>
-  </si>
-  <si>
     <t>Tuxo4459</t>
+  </si>
+  <si>
+    <t>RickG@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>DarylD@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>CarlG@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>GlennR@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>MaggieG@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>HershelG@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>Michonne@TestIncidentQueue.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>P@ssw0rd1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,13 +106,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,72 +397,82 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="42.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
+    <hyperlink ref="B1" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Core plumbing is in place with a basic navigation pattern. Will continue building off of this base.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\WhitepaperPerformance\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Magenic\Clients\Xamarin\Repos\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Labo0749</t>
   </si>
@@ -66,13 +66,28 @@
   </si>
   <si>
     <t>P@ssw0rd1</t>
+  </si>
+  <si>
+    <t>MrG4459!</t>
+  </si>
+  <si>
+    <t>New Pwd</t>
+  </si>
+  <si>
+    <t>Orig Pwd</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Normal User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,13 +103,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,9 +139,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -394,85 +424,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7265625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7"/>
-    <hyperlink ref="B1" r:id="rId8"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#18 Initial work on the performance dashboard.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Magenic\Clients\Xamarin\Repos\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\WhitepaperPerformance\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Labo0749</t>
-  </si>
-  <si>
     <t>Zuwu5875</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Normal User</t>
+  </si>
+  <si>
+    <t>P@ssw0rd2</t>
   </si>
 </sst>
 </file>
@@ -426,92 +426,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Safety check - pre fetch from Dev.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Labo0749</t>
   </si>
@@ -81,24 +81,19 @@
   </si>
   <si>
     <t>Normal User</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,17 +130,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,7 +418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -435,13 +429,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -449,7 +443,10 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -489,8 +486,14 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" t="s">
         <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,10 +511,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Safety checking - login working under iOS and still much to do with Dashboard.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\WhitepaperPerformance\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Magenic\Clients\Xamarin\Repos\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Zuwu5875</t>
   </si>
@@ -81,24 +81,19 @@
   </si>
   <si>
     <t>P@ssw0rd2</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,17 +130,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,44 +418,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -471,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -479,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -487,15 +480,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -510,12 +509,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#32 completion of work on Worker Queue Screen.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Magenic\Clients\Xamarin\Repos\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\WhitepaperPerformance\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>Zuwu5875</t>
   </si>
   <si>
-    <t>Pufa7292</t>
-  </si>
-  <si>
     <t>Hoyo4800</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Manager</t>
+  </si>
+  <si>
+    <t>P@ssw0rd4</t>
   </si>
 </sst>
 </file>
@@ -418,98 +418,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to the storyboard layout and constraints to fix some UI irregularities with the iOS app.
</commit_message>
<xml_diff>
--- a/Documents/TestUsers.xlsx
+++ b/Documents/TestUsers.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,14 +138,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,7 +430,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,8 +457,8 @@
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -513,8 +524,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>